<commit_message>
see blog dev entry #12
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -100,6 +100,15 @@
   <si>
     <t>((knowledge+1) / (knowledge + 6.000f)) * Youthfulness() * 30
 max 25%</t>
+  </si>
+  <si>
+    <t>AOE Dmg/second</t>
+  </si>
+  <si>
+    <t>deals dmg around the MC</t>
+  </si>
+  <si>
+    <t>aoeLvl * Wisdom/5000</t>
   </si>
 </sst>
 </file>
@@ -195,30 +204,30 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -527,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,8 +581,8 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="10"/>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -584,123 +593,161 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="9"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>10</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:9" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>16</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
+  <mergeCells count="32">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
@@ -717,17 +764,6 @@
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
lifesteal, boss1 tile, floor progression
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t>ID</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>armour</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Life Steal</t>
   </si>
 </sst>
 </file>
@@ -258,23 +264,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -582,9 +588,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D24" sqref="D24:D25"/>
     </sheetView>
   </sheetViews>
@@ -627,7 +633,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
@@ -639,29 +645,29 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="11" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
@@ -754,9 +760,9 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
@@ -884,35 +890,51 @@
       <c r="C25" s="7"/>
       <c r="D25" s="8"/>
     </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:C5"/>
+  <mergeCells count="63">
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
@@ -926,25 +948,33 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>